<commit_message>
result of experiments on MALDROID with 5, 6, 10, 15, 20 neighbors
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5818A89E-96D4-40CF-B64C-829DC25C78DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D19C6-D8A3-4429-81B0-475682B9FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="3" activeTab="5" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Sperimentazioni 5 vicini" sheetId="2" r:id="rId2"/>
+    <sheet name="Sperimentazioni 6 vicini 250 ep" sheetId="3" r:id="rId3"/>
+    <sheet name="Sperimentazioni 10 vicini" sheetId="4" r:id="rId4"/>
+    <sheet name="Sperimentazioni 15 vicini" sheetId="5" r:id="rId5"/>
+    <sheet name="Sperimentazioni 20 vicini" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="65">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -70,12 +75,180 @@
   <si>
     <t>DATASET UNSWNUMERIC
 esempi: 175341</t>
+  </si>
+  <si>
+    <t>train_loss</t>
+  </si>
+  <si>
+    <t>train_accuracy</t>
+  </si>
+  <si>
+    <t>validation_accuracy</t>
+  </si>
+  <si>
+    <t>validation_loss</t>
+  </si>
+  <si>
+    <t>learning_rate</t>
+  </si>
+  <si>
+    <t>train_time</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>dropout_1</t>
+  </si>
+  <si>
+    <t>dropuout_2</t>
+  </si>
+  <si>
+    <t>dropuout_3</t>
+  </si>
+  <si>
+    <t>test_time</t>
+  </si>
+  <si>
+    <t>MALDROID</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>2,6548322 mins</t>
+  </si>
+  <si>
+    <t>3,5428217 mins</t>
+  </si>
+  <si>
+    <t>4,0879505 mins</t>
+  </si>
+  <si>
+    <t>3,9078095 mins</t>
+  </si>
+  <si>
+    <t>4,2934874 mins</t>
+  </si>
+  <si>
+    <t>3,5594298 mins</t>
+  </si>
+  <si>
+    <t>1 layer conv</t>
+  </si>
+  <si>
+    <t>2 layer conv</t>
+  </si>
+  <si>
+    <t>3 layer conv</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>macro avg</t>
+  </si>
+  <si>
+    <t>weighted avg</t>
+  </si>
+  <si>
+    <t>F1 SCORES MALDROID</t>
+  </si>
+  <si>
+    <t>train set</t>
+  </si>
+  <si>
+    <t>validation set</t>
+  </si>
+  <si>
+    <t>test set</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>5,27 mins</t>
+  </si>
+  <si>
+    <t>3,24 mins</t>
+  </si>
+  <si>
+    <t>7,37 mins</t>
+  </si>
+  <si>
+    <t>1,77 mins</t>
+  </si>
+  <si>
+    <t>0,63 mins</t>
+  </si>
+  <si>
+    <t>1,43 mins</t>
+  </si>
+  <si>
+    <t>8,51 mins</t>
+  </si>
+  <si>
+    <t>3,01 mins</t>
+  </si>
+  <si>
+    <t>3,50 mins</t>
+  </si>
+  <si>
+    <t>1,30 mins</t>
+  </si>
+  <si>
+    <t>4,06 mins</t>
+  </si>
+  <si>
+    <t>4,16 mins</t>
+  </si>
+  <si>
+    <t>5,25 mins</t>
+  </si>
+  <si>
+    <t>5,24 mins</t>
+  </si>
+  <si>
+    <t>5,16 mins</t>
+  </si>
+  <si>
+    <t>4,83 mins</t>
+  </si>
+  <si>
+    <t>4,78 mins</t>
+  </si>
+  <si>
+    <t>4,71 mins</t>
+  </si>
+  <si>
+    <t>4,57 mins</t>
+  </si>
+  <si>
+    <t>4,38 mins</t>
+  </si>
+  <si>
+    <t>4,39 mins</t>
+  </si>
+  <si>
+    <t>4,59 mins</t>
+  </si>
+  <si>
+    <t>3,97 mins</t>
+  </si>
+  <si>
+    <t>3,62 mins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,7 +266,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,15 +274,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -426,7 +616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22EEED4-BDEB-4A88-9141-7C843C6B9F71}">
   <dimension ref="B4:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -768,4 +958,2674 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
+  <dimension ref="A2:O25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.82969999999999999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0755999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.79239999999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.1104000000000001</v>
+      </c>
+      <c r="F6">
+        <v>8.8999999999999995E-4</v>
+      </c>
+      <c r="G6">
+        <v>64</v>
+      </c>
+      <c r="H6">
+        <v>0.12720000000000001</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0.7974</v>
+      </c>
+      <c r="C8">
+        <v>1.1066</v>
+      </c>
+      <c r="D8">
+        <v>0.77949999999999997</v>
+      </c>
+      <c r="E8">
+        <v>1.1231</v>
+      </c>
+      <c r="F8">
+        <v>3.3E-4</v>
+      </c>
+      <c r="G8">
+        <v>64</v>
+      </c>
+      <c r="H8">
+        <v>0.42820000000000003</v>
+      </c>
+      <c r="I8">
+        <v>0.2611</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>0.78049999999999997</v>
+      </c>
+      <c r="C10">
+        <v>1.1236999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.75549999999999995</v>
+      </c>
+      <c r="E10">
+        <v>1.1452</v>
+      </c>
+      <c r="F10">
+        <v>6.7000000000000002E-4</v>
+      </c>
+      <c r="G10">
+        <v>64</v>
+      </c>
+      <c r="H10">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.25640000000000002</v>
+      </c>
+      <c r="J10">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="D17">
+        <v>0.753</v>
+      </c>
+      <c r="E17">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="G17">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="H17">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="I17">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="K17">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L17">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="M17">
+        <v>0.80600000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="D18">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="E18">
+        <v>0.443</v>
+      </c>
+      <c r="G18">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="I18">
+        <v>0.495</v>
+      </c>
+      <c r="K18">
+        <v>0.621</v>
+      </c>
+      <c r="L18">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="M18">
+        <v>0.50600000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0.76</v>
+      </c>
+      <c r="D19">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="G19">
+        <v>0.746</v>
+      </c>
+      <c r="H19">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="I19">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="K19">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="L19">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="M19">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="D20">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.877</v>
+      </c>
+      <c r="I20">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="K20">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="L20">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="M20">
+        <v>0.70899999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="D21">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="G21">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="H21">
+        <v>0.78</v>
+      </c>
+      <c r="I21">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="K21">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L21">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="M21">
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="D23">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="E23">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="H23">
+        <v>0.78</v>
+      </c>
+      <c r="I23">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="K23">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="L23">
+        <v>0.754</v>
+      </c>
+      <c r="M23">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="D24">
+        <v>0.753</v>
+      </c>
+      <c r="E24">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="G24">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="H24">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="K24">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="L24">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="M24">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="D25">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="E25">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="H25">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="I25">
+        <v>0.621</v>
+      </c>
+      <c r="K25">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="L25">
+        <v>0.751</v>
+      </c>
+      <c r="M25">
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B105D77C-7A91-4CF2-88E5-870B419B2DCC}">
+  <dimension ref="A2:O25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.84809999999999997</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0579000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="E6">
+        <v>1.0967</v>
+      </c>
+      <c r="F6">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="G6">
+        <v>64</v>
+      </c>
+      <c r="H6">
+        <v>0.16950000000000001</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0.8377</v>
+      </c>
+      <c r="C8">
+        <v>1.0673999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="E8">
+        <v>1.0995999999999999</v>
+      </c>
+      <c r="F8">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="G8">
+        <v>128</v>
+      </c>
+      <c r="H8">
+        <v>0.127</v>
+      </c>
+      <c r="I8">
+        <v>0.37930000000000003</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>0.7954</v>
+      </c>
+      <c r="C10">
+        <v>1.109</v>
+      </c>
+      <c r="D10">
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="E10">
+        <v>1.1428</v>
+      </c>
+      <c r="F10">
+        <v>9.2000000000000003E-4</v>
+      </c>
+      <c r="G10">
+        <v>64</v>
+      </c>
+      <c r="H10">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="I10">
+        <v>7.9600000000000004E-2</v>
+      </c>
+      <c r="J10">
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.85</v>
+      </c>
+      <c r="D17">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="E17">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="G17">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="H17">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="I17">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K17">
+        <v>0.83</v>
+      </c>
+      <c r="L17">
+        <v>0.78</v>
+      </c>
+      <c r="M17">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="D18">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="E18">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G18">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="H18">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="I18">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="K18">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="L18">
+        <v>0.59</v>
+      </c>
+      <c r="M18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="D19">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H19">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="I19">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="K19">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="L19">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="M19">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="D20">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G20">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="H20">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="I20">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="K20">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="L20">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="M20">
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="D21">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E21">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="G21">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="H21">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="I21">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="K21">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="L21">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="M21">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="D23">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="E23">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.84</v>
+      </c>
+      <c r="H23">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="I23">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="K23">
+        <v>0.8</v>
+      </c>
+      <c r="L23">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="M23">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D24">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="E24">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="H24">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="I24">
+        <v>0.54</v>
+      </c>
+      <c r="K24">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="L24">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="M24">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="D25">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="E25">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="H25">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="I25">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="K25">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="L25">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="M25">
+        <v>0.624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779C6AFA-6852-46CD-A347-3A6A077B5816}">
+  <dimension ref="A2:O25"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0871999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.78810000000000002</v>
+      </c>
+      <c r="E6">
+        <v>1.1164000000000001</v>
+      </c>
+      <c r="F6">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="G6">
+        <v>128</v>
+      </c>
+      <c r="H6">
+        <v>0.17780000000000001</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0.78259999999999996</v>
+      </c>
+      <c r="C8">
+        <v>1.1223000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="E8">
+        <v>1.1434</v>
+      </c>
+      <c r="F8">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="G8">
+        <v>512</v>
+      </c>
+      <c r="H8">
+        <v>0.3261</v>
+      </c>
+      <c r="I8">
+        <v>0.50190000000000001</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>0.77590000000000003</v>
+      </c>
+      <c r="C10">
+        <v>1.1282000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="E10">
+        <v>1.1560999999999999</v>
+      </c>
+      <c r="F10">
+        <v>8.8000000000000003E-4</v>
+      </c>
+      <c r="G10">
+        <v>256</v>
+      </c>
+      <c r="H10">
+        <v>0.1832</v>
+      </c>
+      <c r="I10">
+        <v>0.62929999999999997</v>
+      </c>
+      <c r="J10">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="D17">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="E17">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="G17">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="H17">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="I17">
+        <v>0.8</v>
+      </c>
+      <c r="K17">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="L17">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="M17">
+        <v>0.80900000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="H18">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="I18">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="K18">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="L18">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="M18">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="E19">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="H19">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="I19">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="K19">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L19">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="M19">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="D20">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="G20">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="H20">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="K20">
+        <v>0.877</v>
+      </c>
+      <c r="L20">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="M20">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.81</v>
+      </c>
+      <c r="D21">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G21">
+        <v>0.749</v>
+      </c>
+      <c r="H21">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="I21">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="K21">
+        <v>0.753</v>
+      </c>
+      <c r="L21">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="M21">
+        <v>0.68100000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D23">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="E23">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H23">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="I23">
+        <v>0.65</v>
+      </c>
+      <c r="K23">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="L23">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="M23">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="D24">
+        <v>0.751</v>
+      </c>
+      <c r="E24">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.745</v>
+      </c>
+      <c r="H24">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="I24">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="K24">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="L24">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="M24">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D25">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="E25">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="H25">
+        <v>0.751</v>
+      </c>
+      <c r="I25">
+        <v>0.62</v>
+      </c>
+      <c r="K25">
+        <v>0.77</v>
+      </c>
+      <c r="L25">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="M25">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11B797D-C90C-4817-BCDE-D007EA2B0243}">
+  <dimension ref="A2:O25"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.83</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0741000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.79859999999999998</v>
+      </c>
+      <c r="E6">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="F6">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="G6">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="C8">
+        <v>1.1254</v>
+      </c>
+      <c r="D8">
+        <v>0.77029999999999998</v>
+      </c>
+      <c r="E8">
+        <v>1.1336999999999999</v>
+      </c>
+      <c r="F8">
+        <v>7.2000000000000005E-4</v>
+      </c>
+      <c r="G8">
+        <v>128</v>
+      </c>
+      <c r="H8">
+        <v>0.51239999999999997</v>
+      </c>
+      <c r="I8">
+        <v>0.34260000000000002</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="C10">
+        <v>1.1335</v>
+      </c>
+      <c r="D10">
+        <v>0.75360000000000005</v>
+      </c>
+      <c r="E10">
+        <v>1.1472</v>
+      </c>
+      <c r="F10">
+        <v>3.8000000000000002E-4</v>
+      </c>
+      <c r="G10">
+        <v>128</v>
+      </c>
+      <c r="H10">
+        <v>0.2235</v>
+      </c>
+      <c r="I10">
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.12180000000000001</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="D17">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="E17">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="G17">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="H17">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="I17">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="K17">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="L17">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="M17">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="D18">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="G18">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="H18">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="I18">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="K18">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="L18">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="M18">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="E19">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="H19">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="I19">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="L19">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="M19">
+        <v>0.43099999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="D20">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="G20">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="H20">
+        <v>0.871</v>
+      </c>
+      <c r="I20">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="K20">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="L20">
+        <v>0.871</v>
+      </c>
+      <c r="M20">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.84</v>
+      </c>
+      <c r="D21">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="G21">
+        <v>0.745</v>
+      </c>
+      <c r="H21">
+        <v>0.73</v>
+      </c>
+      <c r="I21">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="K21">
+        <v>0.75</v>
+      </c>
+      <c r="L21">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="M21">
+        <v>0.67900000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="D23">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="E23">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="H23">
+        <v>0.76</v>
+      </c>
+      <c r="I23">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="K23">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="L23">
+        <v>0.755</v>
+      </c>
+      <c r="M23">
+        <v>0.52100000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="D24">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0.61</v>
+      </c>
+      <c r="G24">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="H24">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="I24">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="K24">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="L24">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="M24">
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="D25">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E25">
+        <v>0.63</v>
+      </c>
+      <c r="G25">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="H25">
+        <v>0.754</v>
+      </c>
+      <c r="I25">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="K25">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="L25">
+        <v>0.751</v>
+      </c>
+      <c r="M25">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB80A9F-9B2B-4416-875B-051410133169}">
+  <dimension ref="A2:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.80259999999999998</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.1041000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.78380000000000005</v>
+      </c>
+      <c r="E6">
+        <v>1.1247</v>
+      </c>
+      <c r="F6">
+        <v>6.4999999999999997E-4</v>
+      </c>
+      <c r="G6">
+        <v>256</v>
+      </c>
+      <c r="H6">
+        <v>0.12509999999999999</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0.78859999999999997</v>
+      </c>
+      <c r="C8">
+        <v>1.1151</v>
+      </c>
+      <c r="D8">
+        <v>0.77029999999999998</v>
+      </c>
+      <c r="E8">
+        <v>1.1333</v>
+      </c>
+      <c r="F8">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="G8">
+        <v>128</v>
+      </c>
+      <c r="H8">
+        <v>0.1043</v>
+      </c>
+      <c r="I8">
+        <v>8.7900000000000006E-2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>0.75649999999999995</v>
+      </c>
+      <c r="C10">
+        <v>1.147</v>
+      </c>
+      <c r="D10">
+        <v>0.75180000000000002</v>
+      </c>
+      <c r="E10">
+        <v>1.1518999999999999</v>
+      </c>
+      <c r="F10">
+        <v>5.1000000000000004E-4</v>
+      </c>
+      <c r="G10">
+        <v>128</v>
+      </c>
+      <c r="H10">
+        <v>0.49409999999999998</v>
+      </c>
+      <c r="I10">
+        <v>0.1045</v>
+      </c>
+      <c r="J10">
+        <v>0.83760000000000001</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="D17">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.8</v>
+      </c>
+      <c r="G17">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="H17">
+        <v>0.754</v>
+      </c>
+      <c r="I17">
+        <v>0.81</v>
+      </c>
+      <c r="K17">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="L17">
+        <v>0.751</v>
+      </c>
+      <c r="M17">
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="D18">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="E18">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="I18">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="K18">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="L18">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="M18">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="E19">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="G19">
+        <v>0.73</v>
+      </c>
+      <c r="H19">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="I19">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="K19">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="L19">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="M19">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="D20">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E20">
+        <v>0.71</v>
+      </c>
+      <c r="G20">
+        <v>0.879</v>
+      </c>
+      <c r="H20">
+        <v>0.873</v>
+      </c>
+      <c r="I20">
+        <v>0.71</v>
+      </c>
+      <c r="K20">
+        <v>0.871</v>
+      </c>
+      <c r="L20">
+        <v>0.876</v>
+      </c>
+      <c r="M20">
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="D21">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E21">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="G21">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="H21">
+        <v>0.746</v>
+      </c>
+      <c r="I21">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="K21">
+        <v>0.753</v>
+      </c>
+      <c r="L21">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="M21">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="D23">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="E23">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="G23">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="H23">
+        <v>0.77</v>
+      </c>
+      <c r="I23">
+        <v>0.66</v>
+      </c>
+      <c r="K23">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="L23">
+        <v>0.75</v>
+      </c>
+      <c r="M23">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="D24">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="E24">
+        <v>0.59</v>
+      </c>
+      <c r="G24">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="H24">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="I24">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="K24">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="L24">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="M24">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D25">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E25">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="H25">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I25">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="K25">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="L25">
+        <v>0.745</v>
+      </c>
+      <c r="M25">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
result of experiments on MALDROID with 100 neighbors 1 layer conv
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D19C6-D8A3-4429-81B0-475682B9FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E91832-7127-43EF-ACE5-60FFB3AE2FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="3" activeTab="5" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="4" activeTab="6" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sperimentazioni 10 vicini" sheetId="4" r:id="rId4"/>
     <sheet name="Sperimentazioni 15 vicini" sheetId="5" r:id="rId5"/>
     <sheet name="Sperimentazioni 20 vicini" sheetId="6" r:id="rId6"/>
+    <sheet name="Sperimentazioni 100 vicini" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="67">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -240,6 +241,12 @@
   </si>
   <si>
     <t>3,62 mins</t>
+  </si>
+  <si>
+    <t>4,22 mins</t>
+  </si>
+  <si>
+    <t>12,36 mins</t>
   </si>
 </sst>
 </file>
@@ -3100,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB80A9F-9B2B-4416-875B-051410133169}">
   <dimension ref="A2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F30" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,4 +3635,335 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CB477A-53CF-4776-A7EB-A1C5CB3DE899}">
+  <dimension ref="A2:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.1101000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.79239999999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.1171</v>
+      </c>
+      <c r="F6">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="G6">
+        <v>256</v>
+      </c>
+      <c r="H6">
+        <v>0.13539999999999999</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="D17">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="E17">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="D18">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D19">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="E19">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="E20">
+        <v>0.71299999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.81</v>
+      </c>
+      <c r="D21">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="E21">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.8</v>
+      </c>
+      <c r="D23">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="E23">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="D24">
+        <v>0.746</v>
+      </c>
+      <c r="E24">
+        <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="D25">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E25">
+        <v>0.626</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
result of experiments on MALDROID with 5 neighbors, after build test graph correction
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E91832-7127-43EF-ACE5-60FFB3AE2FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C459F5-1E5A-431B-B66D-37A4B217B90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="4" activeTab="6" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="68">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -126,15 +126,6 @@
     <t>4,0879505 mins</t>
   </si>
   <si>
-    <t>3,9078095 mins</t>
-  </si>
-  <si>
-    <t>4,2934874 mins</t>
-  </si>
-  <si>
-    <t>3,5594298 mins</t>
-  </si>
-  <si>
     <t>1 layer conv</t>
   </si>
   <si>
@@ -247,6 +238,18 @@
   </si>
   <si>
     <t>12,36 mins</t>
+  </si>
+  <si>
+    <t>test set aggiornato</t>
+  </si>
+  <si>
+    <t>61,08 mins</t>
+  </si>
+  <si>
+    <t>62,16 mins</t>
+  </si>
+  <si>
+    <t>65,82 mins</t>
   </si>
 </sst>
 </file>
@@ -969,10 +972,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
-  <dimension ref="A2:O25"/>
+  <dimension ref="A2:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,25 +985,25 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -1035,12 +1038,12 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.82969999999999999</v>
@@ -1073,19 +1076,19 @@
         <v>23</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="M6">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.7974</v>
@@ -1118,19 +1121,19 @@
         <v>24</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="M8">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.78049999999999997</v>
@@ -1163,13 +1166,13 @@
         <v>25</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="M10">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1186,61 +1189,70 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="3"/>
       <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1253,26 +1265,35 @@
       <c r="E17">
         <v>0.80500000000000005</v>
       </c>
-      <c r="G17">
+      <c r="F17">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="H17">
         <v>0.82299999999999995</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.77400000000000002</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.80800000000000005</v>
       </c>
       <c r="K17">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="M17">
         <v>0.82699999999999996</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>0.74399999999999999</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>0.80600000000000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1285,26 +1306,35 @@
       <c r="E18">
         <v>0.443</v>
       </c>
-      <c r="G18">
+      <c r="F18">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="H18">
         <v>0.61299999999999999</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.56299999999999994</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>0.495</v>
       </c>
       <c r="K18">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="M18">
         <v>0.621</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>0.55700000000000005</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>0.50600000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0.56599999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1317,26 +1347,35 @@
       <c r="E19">
         <v>0.33800000000000002</v>
       </c>
-      <c r="G19">
+      <c r="F19">
+        <v>0.753</v>
+      </c>
+      <c r="H19">
         <v>0.746</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>0.70099999999999996</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>0.32300000000000001</v>
       </c>
       <c r="K19">
         <v>0.72099999999999997</v>
       </c>
-      <c r="L19">
+      <c r="M19">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="N19">
         <v>0.66500000000000004</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>0.53400000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>0.70599999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1349,26 +1388,35 @@
       <c r="E20">
         <v>0.72199999999999998</v>
       </c>
-      <c r="G20">
+      <c r="F20">
+        <v>0.92</v>
+      </c>
+      <c r="H20">
         <v>0.88500000000000001</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>0.877</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>0.70699999999999996</v>
       </c>
       <c r="K20">
+        <v>0.875</v>
+      </c>
+      <c r="M20">
         <v>0.88600000000000001</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>0.88200000000000001</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>0.70899999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>0.878</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1381,28 +1429,37 @@
       <c r="E21">
         <v>0.70099999999999996</v>
       </c>
-      <c r="G21">
+      <c r="F21">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="H21">
         <v>0.79400000000000004</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>0.78</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>0.66400000000000003</v>
       </c>
       <c r="K21">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="M21">
         <v>0.76700000000000002</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>0.71899999999999997</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>0.68700000000000006</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>0.747</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.82799999999999996</v>
@@ -1413,28 +1470,37 @@
       <c r="E23">
         <v>0.65800000000000003</v>
       </c>
-      <c r="G23">
+      <c r="F23">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="H23">
         <v>0.80600000000000005</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>0.78</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.65100000000000002</v>
       </c>
       <c r="K23">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="M23">
         <v>0.79600000000000004</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>0.754</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>0.66400000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.79700000000000004</v>
@@ -1445,28 +1511,37 @@
       <c r="E24">
         <v>0.60199999999999998</v>
       </c>
-      <c r="G24">
+      <c r="F24">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="H24">
         <v>0.77200000000000002</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>0.73899999999999999</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>0.59899999999999998</v>
       </c>
       <c r="K24">
+        <v>0.746</v>
+      </c>
+      <c r="M24">
         <v>0.76400000000000001</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>0.71299999999999997</v>
       </c>
-      <c r="M24">
+      <c r="O24">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.82699999999999996</v>
@@ -1477,23 +1552,32 @@
       <c r="E25">
         <v>0.63100000000000001</v>
       </c>
-      <c r="G25">
+      <c r="F25">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="H25">
         <v>0.80100000000000005</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.77400000000000002</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>0.621</v>
       </c>
       <c r="K25">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="M25">
         <v>0.79200000000000004</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>0.751</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>0.66500000000000004</v>
+      </c>
+      <c r="P25">
+        <v>0.77400000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1569,12 +1653,12 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.84809999999999997</v>
@@ -1604,10 +1688,10 @@
         <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M6">
         <v>250</v>
@@ -1619,7 +1703,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.8377</v>
@@ -1649,10 +1733,10 @@
         <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M8">
         <v>250</v>
@@ -1664,7 +1748,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.7954</v>
@@ -1694,10 +1778,10 @@
         <v>0.55430000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M10">
         <v>250</v>
@@ -1722,56 +1806,56 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1936,7 +2020,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.85099999999999998</v>
@@ -1968,7 +2052,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.82399999999999995</v>
@@ -2000,7 +2084,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.84899999999999998</v>
@@ -2103,12 +2187,12 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.81799999999999995</v>
@@ -2138,10 +2222,10 @@
         <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M6">
         <v>150</v>
@@ -2153,7 +2237,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.78259999999999996</v>
@@ -2183,10 +2267,10 @@
         <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M8">
         <v>150</v>
@@ -2198,7 +2282,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.77590000000000003</v>
@@ -2228,10 +2312,10 @@
         <v>4.0599999999999997E-2</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M10">
         <v>150</v>
@@ -2256,56 +2340,56 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2470,7 +2554,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.81899999999999995</v>
@@ -2502,7 +2586,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.78600000000000003</v>
@@ -2534,7 +2618,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.81499999999999995</v>
@@ -2637,12 +2721,12 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.83</v>
@@ -2672,10 +2756,10 @@
         <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M6">
         <v>150</v>
@@ -2687,7 +2771,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.77800000000000002</v>
@@ -2717,10 +2801,10 @@
         <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M8">
         <v>150</v>
@@ -2732,7 +2816,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.77200000000000002</v>
@@ -2762,10 +2846,10 @@
         <v>0.12180000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M10">
         <v>150</v>
@@ -2790,56 +2874,56 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3004,7 +3088,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.83599999999999997</v>
@@ -3036,7 +3120,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.80400000000000005</v>
@@ -3068,7 +3152,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.83099999999999996</v>
@@ -3171,12 +3255,12 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.80259999999999998</v>
@@ -3206,10 +3290,10 @@
         <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M6">
         <v>150</v>
@@ -3221,7 +3305,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>0.78859999999999997</v>
@@ -3251,10 +3335,10 @@
         <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="M8">
         <v>150</v>
@@ -3266,7 +3350,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.75649999999999995</v>
@@ -3296,10 +3380,10 @@
         <v>0.83760000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M10">
         <v>150</v>
@@ -3324,56 +3408,56 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3538,7 +3622,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.80400000000000005</v>
@@ -3570,7 +3654,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.76400000000000001</v>
@@ -3602,7 +3686,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.79800000000000004</v>
@@ -3641,7 +3725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CB477A-53CF-4776-A7EB-A1C5CB3DE899}">
   <dimension ref="A2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -3705,12 +3789,12 @@
         <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>0.79730000000000001</v>
@@ -3740,10 +3824,10 @@
         <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M6">
         <v>150</v>
@@ -3755,7 +3839,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>22</v>
@@ -3772,7 +3856,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -3799,56 +3883,56 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3923,7 +4007,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0.8</v>
@@ -3937,7 +4021,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>0.75800000000000001</v>
@@ -3951,7 +4035,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0.79300000000000004</v>

</xml_diff>

<commit_message>
result experiments after train corrections
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C459F5-1E5A-431B-B66D-37A4B217B90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C090FDCD-2143-4347-84C5-09D091A31E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="76">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -250,6 +250,30 @@
   </si>
   <si>
     <t>65,82 mins</t>
+  </si>
+  <si>
+    <t>F1 SCORES MALDROID AFTER TRAIN CORRECTION</t>
+  </si>
+  <si>
+    <t>MALDROID AFTER TRAIN CORRECTION</t>
+  </si>
+  <si>
+    <t>3,48 mins</t>
+  </si>
+  <si>
+    <t>0,38 mins</t>
+  </si>
+  <si>
+    <t>6,65 mins</t>
+  </si>
+  <si>
+    <t>63,71 mins</t>
+  </si>
+  <si>
+    <t>66,70 mins</t>
+  </si>
+  <si>
+    <t>60,93 mins</t>
   </si>
 </sst>
 </file>
@@ -259,7 +283,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,13 +291,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -297,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -310,6 +346,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -972,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
-  <dimension ref="A2:P25"/>
+  <dimension ref="A2:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +1026,7 @@
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
@@ -1173,21 +1211,21 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1252,7 +1290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1293,7 +1331,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1334,7 +1372,7 @@
         <v>0.56599999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1375,7 +1413,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1416,7 +1454,7 @@
         <v>0.878</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1457,7 +1495,7 @@
         <v>0.747</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -1498,7 +1536,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1539,7 +1577,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1578,6 +1616,527 @@
       </c>
       <c r="P25">
         <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>0.8145</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1.0987</v>
+      </c>
+      <c r="D33">
+        <v>0.79679999999999995</v>
+      </c>
+      <c r="E33">
+        <v>1.1066</v>
+      </c>
+      <c r="F33">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M33">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>0.78820000000000001</v>
+      </c>
+      <c r="C35">
+        <v>1.1173999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.76719999999999999</v>
+      </c>
+      <c r="E35">
+        <v>1.1371</v>
+      </c>
+      <c r="F35">
+        <v>8.7000000000000001E-4</v>
+      </c>
+      <c r="G35">
+        <v>512</v>
+      </c>
+      <c r="H35">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="I35">
+        <v>0.186</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>0.78510000000000002</v>
+      </c>
+      <c r="C37">
+        <v>1.1198999999999999</v>
+      </c>
+      <c r="D37">
+        <v>0.75919999999999999</v>
+      </c>
+      <c r="E37">
+        <v>1.1445000000000001</v>
+      </c>
+      <c r="F37">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="G37">
+        <v>32</v>
+      </c>
+      <c r="H37">
+        <v>0.108</v>
+      </c>
+      <c r="I37">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="J37">
+        <v>0.61170000000000002</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="D44">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="E44">
+        <v>0.82</v>
+      </c>
+      <c r="G44">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="H44">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I44">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="K44">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="L44">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="M44">
+        <v>0.80700000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="D45">
+        <v>0.61</v>
+      </c>
+      <c r="E45">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G45">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="H45">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="I45">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="K45">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="L45">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="M45">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>0.752</v>
+      </c>
+      <c r="D46">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E46">
+        <v>0.746</v>
+      </c>
+      <c r="G46">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="H46">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="I46">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="K46">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="L46">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="M46">
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="D47">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="E47">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="G47">
+        <v>0.88</v>
+      </c>
+      <c r="H47">
+        <v>0.88</v>
+      </c>
+      <c r="I47">
+        <v>0.876</v>
+      </c>
+      <c r="K47">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="L47">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="M47">
+        <v>0.85899999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D48">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="E48">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G48">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="H48">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="I48">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="K48">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L48">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="M48">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D50">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="E50">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="G50">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="H50">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I50">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="K50">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="L50">
+        <v>0.753</v>
+      </c>
+      <c r="M50">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>0.79</v>
+      </c>
+      <c r="D51">
+        <v>0.752</v>
+      </c>
+      <c r="E51">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="G51">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="H51">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="I51">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="K51">
+        <v>0.755</v>
+      </c>
+      <c r="L51">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="M51">
+        <v>0.73799999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D52">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="E52">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G52">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="H52">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="I52">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K52">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="L52">
+        <v>0.748</v>
+      </c>
+      <c r="M52">
+        <v>0.76700000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results of experiments with similarity threshold at 0
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C090FDCD-2143-4347-84C5-09D091A31E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AB0895-2263-41EE-913B-18616A669386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="9555" yWindow="390" windowWidth="28845" windowHeight="13890" firstSheet="1" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="84">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -274,6 +274,30 @@
   </si>
   <si>
     <t>60,93 mins</t>
+  </si>
+  <si>
+    <t>MALDROID 0,0 SIMILARITY</t>
+  </si>
+  <si>
+    <t>4,04 mins</t>
+  </si>
+  <si>
+    <t>1,13 mins</t>
+  </si>
+  <si>
+    <t>2,97 mins</t>
+  </si>
+  <si>
+    <t>225,68 mins</t>
+  </si>
+  <si>
+    <t>417,27 mins</t>
+  </si>
+  <si>
+    <t>334,21 mins</t>
+  </si>
+  <si>
+    <t>F1 SCORES MALDROID 0,0 SIMILARITY</t>
   </si>
 </sst>
 </file>
@@ -298,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +332,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,8 +376,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1010,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
-  <dimension ref="A2:Q52"/>
+  <dimension ref="A2:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1058,7 @@
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
@@ -1210,23 +1240,6 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
@@ -1619,23 +1632,23 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1680,7 +1693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1721,11 +1734,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -1766,11 +1779,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1811,29 +1824,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
         <v>26</v>
@@ -1850,7 +1846,7 @@
       </c>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>36</v>
       </c>
@@ -1883,7 +1879,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -1915,7 +1911,7 @@
         <v>0.80700000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1947,7 +1943,7 @@
         <v>0.56499999999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1979,7 +1975,7 @@
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2011,7 +2007,7 @@
         <v>0.85899999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4</v>
       </c>
@@ -2043,7 +2039,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>29</v>
       </c>
@@ -2075,7 +2071,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>30</v>
       </c>
@@ -2107,7 +2103,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>31</v>
       </c>
@@ -2137,6 +2133,510 @@
       </c>
       <c r="M52">
         <v>0.76700000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1.1053999999999999</v>
+      </c>
+      <c r="D62">
+        <v>0.77890000000000004</v>
+      </c>
+      <c r="E62">
+        <v>1.125</v>
+      </c>
+      <c r="F62">
+        <v>6.2E-4</v>
+      </c>
+      <c r="G62">
+        <v>32</v>
+      </c>
+      <c r="H62">
+        <v>0.19220000000000001</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M62">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64">
+        <v>0.7742</v>
+      </c>
+      <c r="C64">
+        <v>1.1315</v>
+      </c>
+      <c r="D64">
+        <v>0.75990000000000002</v>
+      </c>
+      <c r="E64">
+        <v>1.1455</v>
+      </c>
+      <c r="F64">
+        <v>3.8000000000000002E-4</v>
+      </c>
+      <c r="G64">
+        <v>256</v>
+      </c>
+      <c r="H64">
+        <v>0.30409999999999998</v>
+      </c>
+      <c r="I64">
+        <v>0.62219999999999998</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M64">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66">
+        <v>0.75890000000000002</v>
+      </c>
+      <c r="C66">
+        <v>1.1432</v>
+      </c>
+      <c r="D66">
+        <v>0.75119999999999998</v>
+      </c>
+      <c r="E66">
+        <v>1.1543000000000001</v>
+      </c>
+      <c r="F66">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G66">
+        <v>64</v>
+      </c>
+      <c r="H66">
+        <v>0.15490000000000001</v>
+      </c>
+      <c r="I66">
+        <v>8.9700000000000002E-2</v>
+      </c>
+      <c r="J66">
+        <v>0.53120000000000001</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L66" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M66">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M71" s="3"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M72" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="D73">
+        <v>0.745</v>
+      </c>
+      <c r="E73">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G73">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="H73">
+        <v>0.749</v>
+      </c>
+      <c r="I73">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="K73">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="L73">
+        <v>0.747</v>
+      </c>
+      <c r="M73">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D74">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="E74">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="G74">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="H74">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="I74">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K74">
+        <v>0.53</v>
+      </c>
+      <c r="L74">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="M74">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="D75">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="E75">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="G75">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="H75">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="I75">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="K75">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="L75">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="M75">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="D76">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E76">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="G76">
+        <v>0.874</v>
+      </c>
+      <c r="H76">
+        <v>0.872</v>
+      </c>
+      <c r="I76">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="K76">
+        <v>0.86</v>
+      </c>
+      <c r="L76">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="M76">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="D77">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="E77">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="G77">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="H77">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="I77">
+        <v>0.74</v>
+      </c>
+      <c r="K77">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="L77">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="M77">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="D79">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="E79">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="G79">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="H79">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="I79">
+        <v>0.76</v>
+      </c>
+      <c r="K79">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="L79">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="M79">
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="D80">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="E80">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="G80">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="H80">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="I80">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="K80">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="L80">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="M80">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D81">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="E81">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G81">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="H81">
+        <v>0.753</v>
+      </c>
+      <c r="I81">
+        <v>0.752</v>
+      </c>
+      <c r="K81">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L81">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="M81">
+        <v>0.73899999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results of experiments with 10 neighbors with updated train
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AB0895-2263-41EE-913B-18616A669386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3210391A-9248-4C22-9172-CE48CAEA3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="390" windowWidth="28845" windowHeight="13890" firstSheet="1" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="19095" yWindow="10440" windowWidth="19410" windowHeight="10545" firstSheet="2" activeTab="3" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="89">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -298,6 +298,21 @@
   </si>
   <si>
     <t>F1 SCORES MALDROID 0,0 SIMILARITY</t>
+  </si>
+  <si>
+    <t>2,83 mins</t>
+  </si>
+  <si>
+    <t>105,49 mins</t>
+  </si>
+  <si>
+    <t>2,15 mins</t>
+  </si>
+  <si>
+    <t>106,62 mins</t>
+  </si>
+  <si>
+    <t>123,42 mins</t>
   </si>
 </sst>
 </file>
@@ -363,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -378,6 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1042,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
   <dimension ref="A2:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3180,10 +3196,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779C6AFA-6852-46CD-A347-3A6A077B5816}">
-  <dimension ref="A2:O25"/>
+  <dimension ref="A2:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,12 +3222,12 @@
     <col min="16" max="16" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -3249,7 +3265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3290,11 +3306,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3335,11 +3351,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3380,29 +3396,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>26</v>
@@ -3419,7 +3418,7 @@
       </c>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3515,7 +3514,7 @@
         <v>0.48799999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3579,7 +3578,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>0.68100000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -3643,7 +3642,7 @@
         <v>0.52400000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -3675,7 +3674,7 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -3705,6 +3704,507 @@
       </c>
       <c r="M25">
         <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>0.80640000000000001</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1.0992</v>
+      </c>
+      <c r="D33">
+        <v>0.79369999999999996</v>
+      </c>
+      <c r="E33">
+        <v>1.1142000000000001</v>
+      </c>
+      <c r="F33">
+        <v>4.2000000000000002E-4</v>
+      </c>
+      <c r="G33">
+        <v>64</v>
+      </c>
+      <c r="H33">
+        <v>0.26939999999999997</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M33">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>0.8044</v>
+      </c>
+      <c r="C35">
+        <v>1.1013999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.78759999999999997</v>
+      </c>
+      <c r="E35">
+        <v>1.1198999999999999</v>
+      </c>
+      <c r="F35">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="G35">
+        <v>512</v>
+      </c>
+      <c r="H35">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="I35">
+        <v>5.16E-2</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>0.76910000000000001</v>
+      </c>
+      <c r="C37">
+        <v>1.135</v>
+      </c>
+      <c r="D37">
+        <v>0.75370000000000004</v>
+      </c>
+      <c r="E37">
+        <v>1.1485000000000001</v>
+      </c>
+      <c r="F37">
+        <v>4.2000000000000002E-4</v>
+      </c>
+      <c r="G37">
+        <v>128</v>
+      </c>
+      <c r="H37">
+        <v>0.35139999999999999</v>
+      </c>
+      <c r="I37">
+        <v>0.67410000000000003</v>
+      </c>
+      <c r="J37">
+        <v>0.5786</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M37">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M42" s="3"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D44">
+        <v>0.75</v>
+      </c>
+      <c r="E44">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="G44">
+        <v>0.82</v>
+      </c>
+      <c r="H44">
+        <v>0.76</v>
+      </c>
+      <c r="I44">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="K44">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="L44">
+        <v>0.755</v>
+      </c>
+      <c r="M44">
+        <v>0.79300000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>0.62</v>
+      </c>
+      <c r="D45">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="E45">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="G45">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="H45">
+        <v>0.53</v>
+      </c>
+      <c r="I45">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="K45">
+        <v>0.54</v>
+      </c>
+      <c r="L45">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M45">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>0.747</v>
+      </c>
+      <c r="D46">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="E46">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="G46">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="H46">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="I46">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="K46">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="L46">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="M46">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="D47">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="E47">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="G47">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="H47">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="I47">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="K47">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="L47">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="M47">
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="D48">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E48">
+        <v>0.8</v>
+      </c>
+      <c r="G48">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="H48">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="I48">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="K48">
+        <v>0.746</v>
+      </c>
+      <c r="L48">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="M48">
+        <v>0.69899999999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="D50">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="E50">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="G50">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="H50">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="I50">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="K50">
+        <v>0.77</v>
+      </c>
+      <c r="L50">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="M50">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="D51">
+        <v>0.745</v>
+      </c>
+      <c r="E51">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="G51">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="H51">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="I51">
+        <v>0.745</v>
+      </c>
+      <c r="K51">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="L51">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="M51">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="D52">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="E52">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="G52">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="H52">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="I52">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="K52">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="L52">
+        <v>0.753</v>
+      </c>
+      <c r="M52">
+        <v>0.74199999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
results of experiments with 5 neighbors with MALDROID-GAT and MALMEM-GAT
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3210391A-9248-4C22-9172-CE48CAEA3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C288DC02-5A80-4666-AFD7-EC1A53201A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="10440" windowWidth="19410" windowHeight="10545" firstSheet="2" activeTab="3" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="101">
   <si>
     <t>Esempi isolati</t>
   </si>
@@ -313,6 +313,42 @@
   </si>
   <si>
     <t>123,42 mins</t>
+  </si>
+  <si>
+    <t>GCN</t>
+  </si>
+  <si>
+    <t>GAT</t>
+  </si>
+  <si>
+    <t>MALMEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1 SCORES </t>
+  </si>
+  <si>
+    <t>7,16 mins</t>
+  </si>
+  <si>
+    <t>103,03 mins</t>
+  </si>
+  <si>
+    <t>9,25 mins</t>
+  </si>
+  <si>
+    <t>7,56 mins</t>
+  </si>
+  <si>
+    <t>61,79 mins</t>
+  </si>
+  <si>
+    <t>62,64 mins</t>
+  </si>
+  <si>
+    <t>55,93 hours</t>
+  </si>
+  <si>
+    <t>59,07 hours</t>
   </si>
 </sst>
 </file>
@@ -322,7 +358,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +368,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -346,18 +391,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -374,11 +417,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -391,12 +460,25 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Cella da controllare" xfId="2" builtinId="23"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valore non valido" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1056,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
-  <dimension ref="A2:Q81"/>
+  <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" topLeftCell="B99" workbookViewId="0">
+      <selection activeCell="K124" sqref="K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,6 +1164,11 @@
     <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
@@ -1647,7 +1734,8 @@
         <v>0.77400000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1666,6 +1754,11 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
+    <row r="28" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
@@ -2055,7 +2148,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>29</v>
       </c>
@@ -2087,7 +2180,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>30</v>
       </c>
@@ -2119,7 +2212,7 @@
         <v>0.73799999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>31</v>
       </c>
@@ -2151,508 +2244,1260 @@
         <v>0.76700000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="54" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>11</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C58" t="s">
         <v>10</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D58" t="s">
         <v>12</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E58" t="s">
         <v>13</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F58" t="s">
         <v>14</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G58" t="s">
         <v>16</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H58" t="s">
         <v>17</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I58" t="s">
         <v>18</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J58" t="s">
         <v>19</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K58" t="s">
         <v>15</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L58" t="s">
         <v>20</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>26</v>
       </c>
-      <c r="B62">
+      <c r="B61">
         <v>0.79800000000000004</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C61" s="4">
         <v>1.1053999999999999</v>
       </c>
-      <c r="D62">
+      <c r="D61">
         <v>0.77890000000000004</v>
       </c>
-      <c r="E62">
+      <c r="E61">
         <v>1.125</v>
       </c>
-      <c r="F62">
+      <c r="F61">
         <v>6.2E-4</v>
       </c>
-      <c r="G62">
+      <c r="G61">
         <v>32</v>
       </c>
-      <c r="H62">
+      <c r="H61">
         <v>0.19220000000000001</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="I61" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J62" s="3" t="s">
+      <c r="J61" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="K61" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L62" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M62">
+      <c r="M61">
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>27</v>
       </c>
-      <c r="B64">
+      <c r="B63">
         <v>0.7742</v>
       </c>
-      <c r="C64">
+      <c r="C63">
         <v>1.1315</v>
       </c>
-      <c r="D64">
+      <c r="D63">
         <v>0.75990000000000002</v>
       </c>
-      <c r="E64">
+      <c r="E63">
         <v>1.1455</v>
       </c>
-      <c r="F64">
+      <c r="F63">
         <v>3.8000000000000002E-4</v>
       </c>
-      <c r="G64">
+      <c r="G63">
         <v>256</v>
       </c>
-      <c r="H64">
+      <c r="H63">
         <v>0.30409999999999998</v>
       </c>
-      <c r="I64">
+      <c r="I63">
         <v>0.62219999999999998</v>
       </c>
-      <c r="J64" s="3" t="s">
+      <c r="J63" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="K63" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="L63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M64">
+      <c r="M63">
         <v>150</v>
       </c>
     </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A65" t="s">
         <v>28</v>
       </c>
-      <c r="B66">
+      <c r="B65">
         <v>0.75890000000000002</v>
       </c>
-      <c r="C66">
+      <c r="C65">
         <v>1.1432</v>
       </c>
-      <c r="D66">
+      <c r="D65">
         <v>0.75119999999999998</v>
       </c>
-      <c r="E66">
+      <c r="E65">
         <v>1.1543000000000001</v>
       </c>
-      <c r="F66">
+      <c r="F65">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="G66">
+      <c r="G65">
         <v>64</v>
       </c>
-      <c r="H66">
+      <c r="H65">
         <v>0.15490000000000001</v>
       </c>
-      <c r="I66">
+      <c r="I65">
         <v>8.9700000000000002E-2</v>
       </c>
-      <c r="J66">
+      <c r="J65">
         <v>0.53120000000000001</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="K65" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="L66" s="2" t="s">
+      <c r="L65" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M66">
+      <c r="M65">
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>83</v>
       </c>
     </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M70" s="3"/>
+    </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C71" s="3"/>
+      <c r="A71" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D71" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="G71" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H71" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I71" s="3"/>
-      <c r="K71" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="L71" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M71" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="M71" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M72" s="3" t="s">
-        <v>35</v>
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="D72">
+        <v>0.745</v>
+      </c>
+      <c r="E72">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G72">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="H72">
+        <v>0.749</v>
+      </c>
+      <c r="I72">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="K72">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="L72">
+        <v>0.747</v>
+      </c>
+      <c r="M72">
+        <v>0.76900000000000002</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C73">
-        <v>0.80600000000000005</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="D73">
-        <v>0.745</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="E73">
-        <v>0.81200000000000006</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="G73">
-        <v>0.78500000000000003</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="H73">
-        <v>0.749</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="I73">
-        <v>0.78100000000000003</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="K73">
-        <v>0.77900000000000003</v>
+        <v>0.53</v>
       </c>
       <c r="L73">
-        <v>0.747</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="M73">
-        <v>0.76900000000000002</v>
+        <v>0.50700000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C74">
-        <v>0.56100000000000005</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="D74">
-        <v>0.52400000000000002</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="E74">
-        <v>0.56299999999999994</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="G74">
-        <v>0.54300000000000004</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="H74">
-        <v>0.54500000000000004</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="I74">
-        <v>0.51700000000000002</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="K74">
-        <v>0.53</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="L74">
-        <v>0.54800000000000004</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="M74">
-        <v>0.50700000000000001</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75">
-        <v>0.73399999999999999</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="D75">
-        <v>0.68600000000000005</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="E75">
-        <v>0.73199999999999998</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="G75">
-        <v>0.72399999999999998</v>
+        <v>0.874</v>
       </c>
       <c r="H75">
-        <v>0.68400000000000005</v>
+        <v>0.872</v>
       </c>
       <c r="I75">
-        <v>0.68600000000000005</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="K75">
-        <v>0.70399999999999996</v>
+        <v>0.86</v>
       </c>
       <c r="L75">
-        <v>0.65200000000000002</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="M75">
-        <v>0.69</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C76">
-        <v>0.90500000000000003</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="D76">
-        <v>0.89600000000000002</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="E76">
-        <v>0.89300000000000002</v>
+        <v>0.81399999999999995</v>
       </c>
       <c r="G76">
-        <v>0.874</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="H76">
-        <v>0.872</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="I76">
-        <v>0.85699999999999998</v>
+        <v>0.74</v>
       </c>
       <c r="K76">
-        <v>0.86</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="L76">
-        <v>0.84899999999999998</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="M76">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>4</v>
-      </c>
-      <c r="C77">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="D77">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="E77">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="G77">
-        <v>0.76100000000000001</v>
-      </c>
-      <c r="H77">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="I77">
-        <v>0.74</v>
-      </c>
-      <c r="K77">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="L77">
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="M77">
         <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="D78">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="E78">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="G78">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="H78">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="I78">
+        <v>0.76</v>
+      </c>
+      <c r="K78">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="L78">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="M78">
+        <v>0.749</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C79">
-        <v>0.80400000000000005</v>
+        <v>0.76100000000000001</v>
       </c>
       <c r="D79">
-        <v>0.77600000000000002</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="E79">
-        <v>0.80400000000000005</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="G79">
-        <v>0.77900000000000003</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="H79">
-        <v>0.75900000000000001</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="I79">
-        <v>0.76</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="K79">
-        <v>0.76800000000000002</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="L79">
-        <v>0.74299999999999999</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="M79">
-        <v>0.749</v>
+        <v>0.70499999999999996</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D80">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="E80">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G80">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="H80">
+        <v>0.753</v>
+      </c>
+      <c r="I80">
+        <v>0.752</v>
+      </c>
+      <c r="K80">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L80">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="M80">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+    </row>
+    <row r="84" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" t="s">
+        <v>17</v>
+      </c>
+      <c r="I86" t="s">
+        <v>18</v>
+      </c>
+      <c r="J86" t="s">
+        <v>19</v>
+      </c>
+      <c r="K86" t="s">
+        <v>15</v>
+      </c>
+      <c r="L86" t="s">
+        <v>20</v>
+      </c>
+      <c r="M86" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>26</v>
+      </c>
+      <c r="B89">
+        <v>0.78539999999999999</v>
+      </c>
+      <c r="C89" s="4">
+        <v>1.1213</v>
+      </c>
+      <c r="D89">
+        <v>0.77159999999999995</v>
+      </c>
+      <c r="E89">
+        <v>1.1352</v>
+      </c>
+      <c r="F89">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="G89">
+        <v>32</v>
+      </c>
+      <c r="H89">
+        <v>0.1769</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M89">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>27</v>
+      </c>
+      <c r="B91">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="C91">
+        <v>1.1167</v>
+      </c>
+      <c r="D91">
+        <v>0.76419999999999999</v>
+      </c>
+      <c r="E91">
+        <v>1.1406000000000001</v>
+      </c>
+      <c r="F91">
+        <v>6.4999999999999997E-4</v>
+      </c>
+      <c r="G91">
+        <v>64</v>
+      </c>
+      <c r="H91">
+        <v>0.13009999999999999</v>
+      </c>
+      <c r="I91">
+        <v>0.1431</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M91">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="D98">
+        <v>0.752</v>
+      </c>
+      <c r="E98">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="G98">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="H98">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="I98">
+        <v>0.81200000000000006</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="D99">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="E99">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="G99">
+        <v>0.626</v>
+      </c>
+      <c r="H99">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I99">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="D100">
+        <v>0.67</v>
+      </c>
+      <c r="E100">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="G100">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="H100">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="I100">
+        <v>0.71399999999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="D101">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="E101">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="G101">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="H101">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="I101">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="D102">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="E102">
+        <v>0.79</v>
+      </c>
+      <c r="G102">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="H102">
+        <v>0.747</v>
+      </c>
+      <c r="I102">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C104">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="D104">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="E104">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="G104">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="H104">
+        <v>0.76</v>
+      </c>
+      <c r="I104">
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C80">
+      <c r="C105">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="D105">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="E105">
+        <v>0.755</v>
+      </c>
+      <c r="G105">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="H105">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="I105">
+        <v>0.73799999999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C106">
+        <v>0.79</v>
+      </c>
+      <c r="D106">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="E106">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="G106">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="H106">
+        <v>0.754</v>
+      </c>
+      <c r="I106">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
+    </row>
+    <row r="109" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" t="s">
+        <v>16</v>
+      </c>
+      <c r="H111" t="s">
+        <v>17</v>
+      </c>
+      <c r="I111" t="s">
+        <v>18</v>
+      </c>
+      <c r="J111" t="s">
+        <v>19</v>
+      </c>
+      <c r="K111" t="s">
+        <v>15</v>
+      </c>
+      <c r="L111" t="s">
+        <v>20</v>
+      </c>
+      <c r="M111" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114">
+        <v>0.75329999999999997</v>
+      </c>
+      <c r="C114" s="4">
+        <v>0.97509999999999997</v>
+      </c>
+      <c r="D114">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E114">
+        <v>0.97740000000000005</v>
+      </c>
+      <c r="F114">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="G114">
+        <v>256</v>
+      </c>
+      <c r="H114">
+        <v>8.1699999999999995E-2</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L114" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M114">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>27</v>
+      </c>
+      <c r="B116">
+        <v>0.75690000000000002</v>
+      </c>
+      <c r="C116">
+        <v>0.97319999999999995</v>
+      </c>
+      <c r="D116">
+        <v>0.75609999999999999</v>
+      </c>
+      <c r="E116">
+        <v>0.97519999999999996</v>
+      </c>
+      <c r="F116">
+        <v>1.2E-4</v>
+      </c>
+      <c r="G116">
+        <v>32</v>
+      </c>
+      <c r="H116">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="I116">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L116" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M116">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3"/>
+      <c r="M121" s="3"/>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="3"/>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>0.999</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>0.999</v>
+      </c>
+      <c r="G123">
+        <v>0.999</v>
+      </c>
+      <c r="H123">
+        <v>0.999</v>
+      </c>
+      <c r="I123">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="C124">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="D124">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E124">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G124">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="H124">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="I124">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2</v>
+      </c>
+      <c r="C125">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="D125">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="E125">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="G125">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H125">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="I125">
+        <v>0.55600000000000005</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>3</v>
+      </c>
+      <c r="C126">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D126">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="E126">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G126">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="H126">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="I126">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C128">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="D128">
+        <v>0.752</v>
+      </c>
+      <c r="E128">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="G128">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="H128">
+        <v>0.753</v>
+      </c>
+      <c r="I128">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C129">
+        <v>0.64</v>
+      </c>
+      <c r="D129">
+        <v>0.624</v>
+      </c>
+      <c r="E129">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="G129">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="H129">
+        <v>0.628</v>
+      </c>
+      <c r="I129">
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130">
+        <v>0.76</v>
+      </c>
+      <c r="D130">
+        <v>0.749</v>
+      </c>
+      <c r="E130">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G130">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="H130">
+        <v>0.752</v>
+      </c>
+      <c r="I130">
         <v>0.76100000000000001</v>
-      </c>
-      <c r="D80">
-        <v>0.72699999999999998</v>
-      </c>
-      <c r="E80">
-        <v>0.76300000000000001</v>
-      </c>
-      <c r="G80">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="H80">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="I80">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="K80">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="L80">
-        <v>0.70299999999999996</v>
-      </c>
-      <c r="M80">
-        <v>0.70499999999999996</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C81">
-        <v>0.79800000000000004</v>
-      </c>
-      <c r="D81">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="E81">
-        <v>0.79800000000000004</v>
-      </c>
-      <c r="G81">
-        <v>0.77300000000000002</v>
-      </c>
-      <c r="H81">
-        <v>0.753</v>
-      </c>
-      <c r="I81">
-        <v>0.752</v>
-      </c>
-      <c r="K81">
-        <v>0.76100000000000001</v>
-      </c>
-      <c r="L81">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="M81">
-        <v>0.73899999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3196,10 +4041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779C6AFA-6852-46CD-A347-3A6A077B5816}">
-  <dimension ref="A2:N52"/>
+  <dimension ref="A2:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3706,21 +4551,27 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -4111,7 +4962,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>29</v>
       </c>
@@ -4143,7 +4994,7 @@
         <v>0.751</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>30</v>
       </c>
@@ -4175,7 +5026,7 @@
         <v>0.70799999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>31</v>
       </c>
@@ -4206,6 +5057,79 @@
       <c r="M52">
         <v>0.74199999999999999</v>
       </c>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C60" s="4"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J62" s="3"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MALMEM new results and results' folder refactoring
</commit_message>
<xml_diff>
--- a/results/Risultati Tesi.xlsx
+++ b/results/Risultati Tesi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\PycharmProjects\TesiMagistrale\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C288DC02-5A80-4666-AFD7-EC1A53201A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA988FA7-4FF4-4056-8D61-5B8CB793D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32460" windowHeight="16575" activeTab="1" xr2:uid="{E6497146-353A-4F0E-9C47-F777002F9586}"/>
   </bookViews>
   <sheets>
     <sheet name="Proprietà Dataset" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -461,9 +461,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1140,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160772B2-DAF4-4F07-8FEB-CBBE25958507}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B99" workbookViewId="0">
-      <selection activeCell="K124" sqref="K124"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1162,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1755,7 +1752,7 @@
       <c r="Q27" s="6"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2262,7 +2259,7 @@
       <c r="N55" s="6"/>
     </row>
     <row r="56" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2769,7 +2766,7 @@
       <c r="N83" s="6"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="8" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3155,7 +3152,7 @@
       <c r="N108" s="6"/>
     </row>
     <row r="109" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="8" t="s">
+      <c r="A109" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3294,7 +3291,7 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -5076,7 +5073,7 @@
       <c r="N54" s="6"/>
     </row>
     <row r="55" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="2"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C60" s="4"/>

</xml_diff>